<commit_message>
More writing and plots
</commit_message>
<xml_diff>
--- a/Documentation/seda2023_codebook_state_updated_202402025.xlsx
+++ b/Documentation/seda2023_codebook_state_updated_202402025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efahle\Dropbox\SEDA\seda_2023\release data\version 2024-02-02\repository files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Downloads\rstudy-edu\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C80DEF-CE33-4548-956B-1FACFA974B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62E449E-34C4-4336-A872-ED3BF4BC2CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38250" yWindow="0" windowWidth="18720" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="seda2023_state_poolsub_gys" sheetId="1" r:id="rId1"/>
@@ -1130,17 +1130,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
-    <col min="5" max="5" width="80.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="80.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>202</v>
       </c>
@@ -1149,7 +1149,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>211</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>197</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>47</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>48</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>49</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>50</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>51</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>52</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>53</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>54</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>55</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>56</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>57</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>58</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>59</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>60</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>61</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>62</v>
       </c>
@@ -2242,17 +2242,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="5" max="5" width="85.88671875" customWidth="1"/>
+    <col min="5" max="5" width="85.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>205</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>212</v>
       </c>
@@ -2270,7 +2270,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>197</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>47</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>48</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>49</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>50</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>51</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>52</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>53</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>54</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>55</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>56</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>57</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>58</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>59</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>60</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>61</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>62</v>
       </c>
@@ -3358,14 +3358,14 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="9.109375" style="1"/>
-    <col min="5" max="5" width="30.33203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="30.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>206</v>
       </c>
@@ -3374,7 +3374,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>207</v>
       </c>
@@ -3383,7 +3383,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>197</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>11</v>
       </c>

</xml_diff>